<commit_message>
Again a few updates
</commit_message>
<xml_diff>
--- a/data/prey_compo_compiled.xlsx
+++ b/data/prey_compo_compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023_09\Analyses\FeSthOpinn\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D951253-DEF6-47A2-9006-A799DC855CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F495FB-3FAB-48E1-9F08-06F209A22C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8C22CE91-C915-4DF3-AAED-2AD3B8EB0434}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="176">
   <si>
     <t>Sp_prey</t>
   </si>
@@ -544,6 +544,27 @@
   </si>
   <si>
     <t>Pinniped (muscle)</t>
+  </si>
+  <si>
+    <t>Pagothenia borchgrevinki</t>
+  </si>
+  <si>
+    <t>Notothenia coriiceps</t>
+  </si>
+  <si>
+    <t>Trematomus bernacchii</t>
+  </si>
+  <si>
+    <t>Trematomus hansoni</t>
+  </si>
+  <si>
+    <t>Trematomus newnesi</t>
+  </si>
+  <si>
+    <t>Trematomus pennellii</t>
+  </si>
+  <si>
+    <t>Goutte et al 2015</t>
   </si>
 </sst>
 </file>
@@ -960,12 +981,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}">
-  <dimension ref="A1:J281"/>
+  <dimension ref="A1:J287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A268" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A271" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="J275" sqref="J275"/>
+      <selection pane="bottomLeft" activeCell="I284" sqref="I284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6390,6 +6411,132 @@
         <v>166</v>
       </c>
     </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A282" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E282">
+        <v>86.8</v>
+      </c>
+      <c r="F282" s="7">
+        <f>E282*0.2</f>
+        <v>17.36</v>
+      </c>
+      <c r="G282">
+        <v>80</v>
+      </c>
+      <c r="I282" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A283" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E283">
+        <v>508</v>
+      </c>
+      <c r="F283" s="7">
+        <f t="shared" ref="F283:F287" si="2">E283*0.2</f>
+        <v>101.60000000000001</v>
+      </c>
+      <c r="G283">
+        <v>80</v>
+      </c>
+      <c r="I283" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A284" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E284">
+        <v>205</v>
+      </c>
+      <c r="F284" s="7">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="G284">
+        <v>80</v>
+      </c>
+      <c r="I284" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A285" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E285">
+        <v>142</v>
+      </c>
+      <c r="F285" s="7">
+        <f t="shared" si="2"/>
+        <v>28.400000000000002</v>
+      </c>
+      <c r="G285">
+        <v>80</v>
+      </c>
+      <c r="I285" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A286" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E286">
+        <v>140</v>
+      </c>
+      <c r="F286" s="7">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="G286">
+        <v>80</v>
+      </c>
+      <c r="I286" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A287" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E287">
+        <v>56.4</v>
+      </c>
+      <c r="F287" s="7">
+        <f t="shared" si="2"/>
+        <v>11.280000000000001</v>
+      </c>
+      <c r="G287">
+        <v>80</v>
+      </c>
+      <c r="I287" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J281" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Change Leopard seal diet
</commit_message>
<xml_diff>
--- a/data/prey_compo_compiled.xlsx
+++ b/data/prey_compo_compiled.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023_09\Analyses\FeSthOpinn\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023_09\01.Analyses\FeSthOpinn\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F495FB-3FAB-48E1-9F08-06F209A22C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB109B8-472F-4115-AB2D-6EE656F5114B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8C22CE91-C915-4DF3-AAED-2AD3B8EB0434}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8C22CE91-C915-4DF3-AAED-2AD3B8EB0434}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$281</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$287</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="178">
   <si>
     <t>Sp_prey</t>
   </si>
@@ -565,6 +565,12 @@
   </si>
   <si>
     <t>Goutte et al 2015</t>
+  </si>
+  <si>
+    <t>Thysanoessa macrura</t>
+  </si>
+  <si>
+    <t>Euphausia crystallorophias</t>
   </si>
 </sst>
 </file>
@@ -981,12 +987,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A271" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A214" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="I284" sqref="I284"/>
+      <selection pane="bottomLeft" activeCell="I244" sqref="I244:I247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1032,7 +1039,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1052,7 +1059,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1072,7 +1079,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
@@ -1089,7 +1096,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
@@ -1106,7 +1113,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>85</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1663,7 +1670,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -1880,7 +1887,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>30</v>
       </c>
@@ -1900,7 +1907,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>30</v>
       </c>
@@ -2040,7 +2047,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
@@ -2060,7 +2067,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>38</v>
       </c>
@@ -2080,7 +2087,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>38</v>
       </c>
@@ -2100,7 +2107,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>38</v>
       </c>
@@ -2140,7 +2147,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -2380,7 +2387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -2440,7 +2447,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>49</v>
       </c>
@@ -2480,7 +2487,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>51</v>
       </c>
@@ -2520,7 +2527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>53</v>
       </c>
@@ -2620,7 +2627,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>57</v>
       </c>
@@ -2840,7 +2847,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>64</v>
       </c>
@@ -2860,7 +2867,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>64</v>
       </c>
@@ -2880,7 +2887,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" s="2" t="s">
         <v>85</v>
       </c>
@@ -3097,7 +3104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>70</v>
       </c>
@@ -3117,7 +3124,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>70</v>
       </c>
@@ -3317,7 +3324,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>53</v>
       </c>
@@ -3338,7 +3345,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>53</v>
       </c>
@@ -3359,7 +3366,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>53</v>
       </c>
@@ -3380,7 +3387,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>76</v>
       </c>
@@ -3401,7 +3408,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>77</v>
       </c>
@@ -3422,7 +3429,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>78</v>
       </c>
@@ -4136,7 +4143,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>93</v>
       </c>
@@ -4159,7 +4166,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>93</v>
       </c>
@@ -4182,7 +4189,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>93</v>
       </c>
@@ -4205,7 +4212,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>93</v>
       </c>
@@ -4228,7 +4235,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>93</v>
       </c>
@@ -4251,7 +4258,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>93</v>
       </c>
@@ -4274,7 +4281,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>93</v>
       </c>
@@ -4297,7 +4304,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>93</v>
       </c>
@@ -4320,7 +4327,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>93</v>
       </c>
@@ -4343,7 +4350,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>93</v>
       </c>
@@ -4366,7 +4373,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>93</v>
       </c>
@@ -4389,7 +4396,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>93</v>
       </c>
@@ -4412,7 +4419,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>93</v>
       </c>
@@ -4435,7 +4442,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>93</v>
       </c>
@@ -4458,7 +4465,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>93</v>
       </c>
@@ -4481,7 +4488,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>93</v>
       </c>
@@ -4504,7 +4511,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>93</v>
       </c>
@@ -4524,7 +4531,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>93</v>
       </c>
@@ -4544,7 +4551,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>93</v>
       </c>
@@ -4564,7 +4571,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>93</v>
       </c>
@@ -4587,7 +4594,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>93</v>
       </c>
@@ -4610,7 +4617,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>93</v>
       </c>
@@ -4633,7 +4640,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>94</v>
       </c>
@@ -4656,7 +4663,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>95</v>
       </c>
@@ -4679,7 +4686,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>96</v>
       </c>
@@ -4702,7 +4709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>97</v>
       </c>
@@ -4725,7 +4732,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>98</v>
       </c>
@@ -4748,7 +4755,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>40</v>
       </c>
@@ -4771,7 +4778,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>93</v>
       </c>
@@ -4795,7 +4802,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>93</v>
       </c>
@@ -4819,7 +4826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>93</v>
       </c>
@@ -4843,7 +4850,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>93</v>
       </c>
@@ -4866,7 +4873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>93</v>
       </c>
@@ -4889,7 +4896,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>93</v>
       </c>
@@ -4912,7 +4919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190"/>
       <c r="B190" t="s">
         <v>100</v>
@@ -4933,7 +4940,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191"/>
       <c r="B191" t="s">
         <v>100</v>
@@ -4954,7 +4961,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192"/>
       <c r="B192" t="s">
         <v>100</v>
@@ -4975,7 +4982,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193"/>
       <c r="B193" t="s">
         <v>100</v>
@@ -4996,7 +5003,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>99</v>
       </c>
@@ -5016,7 +5023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>99</v>
       </c>
@@ -5036,7 +5043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>99</v>
       </c>
@@ -5056,7 +5063,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>99</v>
       </c>
@@ -5076,7 +5083,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>99</v>
       </c>
@@ -5096,7 +5103,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>99</v>
       </c>
@@ -5116,7 +5123,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>99</v>
       </c>
@@ -5136,7 +5143,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>99</v>
       </c>
@@ -5156,7 +5163,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>99</v>
       </c>
@@ -5176,7 +5183,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>99</v>
       </c>
@@ -5196,7 +5203,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>99</v>
       </c>
@@ -5216,7 +5223,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>99</v>
       </c>
@@ -5236,7 +5243,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>99</v>
       </c>
@@ -5256,7 +5263,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>99</v>
       </c>
@@ -5276,7 +5283,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>93</v>
       </c>
@@ -5596,7 +5603,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" s="2" t="s">
         <v>135</v>
       </c>
@@ -5610,7 +5617,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" s="2" t="s">
         <v>136</v>
       </c>
@@ -5624,7 +5631,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
         <v>137</v>
       </c>
@@ -5638,7 +5645,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="2" t="s">
         <v>138</v>
       </c>
@@ -5652,7 +5659,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="2" t="s">
         <v>38</v>
       </c>
@@ -5666,7 +5673,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
         <v>38</v>
       </c>
@@ -5680,7 +5687,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>38</v>
       </c>
@@ -5694,7 +5701,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
         <v>139</v>
       </c>
@@ -5708,7 +5715,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" s="2" t="s">
         <v>140</v>
       </c>
@@ -5722,7 +5729,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" s="2" t="s">
         <v>141</v>
       </c>
@@ -5736,7 +5743,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" s="2" t="s">
         <v>142</v>
       </c>
@@ -5750,7 +5757,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
         <v>143</v>
       </c>
@@ -5764,7 +5771,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
         <v>143</v>
       </c>
@@ -5778,7 +5785,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" s="2" t="s">
         <v>143</v>
       </c>
@@ -5792,7 +5799,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" s="2" t="s">
         <v>70</v>
       </c>
@@ -5806,7 +5813,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
         <v>144</v>
       </c>
@@ -5820,7 +5827,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" s="2" t="s">
         <v>64</v>
       </c>
@@ -5834,7 +5841,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" s="2" t="s">
         <v>145</v>
       </c>
@@ -5848,7 +5855,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" s="2" t="s">
         <v>146</v>
       </c>
@@ -5862,7 +5869,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
         <v>147</v>
       </c>
@@ -5883,7 +5890,7 @@
       <c r="F244" s="7">
         <v>14.9</v>
       </c>
-      <c r="H244" t="s">
+      <c r="I244" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5894,7 +5901,7 @@
       <c r="F245" s="7">
         <v>6.51</v>
       </c>
-      <c r="H245" t="s">
+      <c r="I245" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5905,7 +5912,7 @@
       <c r="F246" s="7">
         <v>5.81</v>
       </c>
-      <c r="H246" t="s">
+      <c r="I246" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5916,11 +5923,11 @@
       <c r="F247" s="7">
         <v>12.3</v>
       </c>
-      <c r="H247" t="s">
+      <c r="I247" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" s="2" t="s">
         <v>93</v>
       </c>
@@ -5934,7 +5941,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" s="2" t="s">
         <v>141</v>
       </c>
@@ -5948,7 +5955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
         <v>38</v>
       </c>
@@ -5962,7 +5969,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" s="2" t="s">
         <v>64</v>
       </c>
@@ -5976,7 +5983,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A252" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="B252" s="2" t="s">
         <v>101</v>
       </c>
@@ -5994,7 +6004,10 @@
         <v>151</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A253" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="B253" s="2" t="s">
         <v>101</v>
       </c>
@@ -6012,7 +6025,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
         <v>93</v>
       </c>
@@ -6033,7 +6046,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>152</v>
       </c>
@@ -6047,7 +6060,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>154</v>
       </c>
@@ -6061,7 +6074,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>154</v>
       </c>
@@ -6075,7 +6088,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>154</v>
       </c>
@@ -6089,7 +6102,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>156</v>
       </c>
@@ -6103,7 +6116,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>152</v>
       </c>
@@ -6117,7 +6130,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>157</v>
       </c>
@@ -6131,7 +6144,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>152</v>
       </c>
@@ -6145,7 +6158,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>152</v>
       </c>
@@ -6159,7 +6172,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>152</v>
       </c>
@@ -6173,7 +6186,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>152</v>
       </c>
@@ -6187,7 +6200,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>156</v>
       </c>
@@ -6201,7 +6214,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>157</v>
       </c>
@@ -6215,7 +6228,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>152</v>
       </c>
@@ -6229,7 +6242,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>157</v>
       </c>
@@ -6243,7 +6256,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>152</v>
       </c>
@@ -6257,7 +6270,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>156</v>
       </c>
@@ -6271,7 +6284,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>152</v>
       </c>
@@ -6285,7 +6298,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>157</v>
       </c>
@@ -6299,7 +6312,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>162</v>
       </c>
@@ -6313,7 +6326,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>162</v>
       </c>
@@ -6327,7 +6340,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>164</v>
       </c>
@@ -6341,7 +6354,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>164</v>
       </c>
@@ -6355,7 +6368,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>164</v>
       </c>
@@ -6369,7 +6382,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>165</v>
       </c>
@@ -6383,7 +6396,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>165</v>
       </c>
@@ -6397,7 +6410,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>165</v>
       </c>
@@ -6538,7 +6551,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J281" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}"/>
+  <autoFilter ref="A1:J287" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Fish"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changing Figure 1 to show difference of Fe release between species at the individual daily level
</commit_message>
<xml_diff>
--- a/data/prey_compo_compiled.xlsx
+++ b/data/prey_compo_compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023_09\01.Analyses\FeSthOpinn\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB109B8-472F-4115-AB2D-6EE656F5114B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB9E7BD-F733-4119-823F-A68BE3E4BB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8C22CE91-C915-4DF3-AAED-2AD3B8EB0434}"/>
   </bookViews>
@@ -987,13 +987,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A214" activePane="bottomLeft"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="I244" sqref="I244:I247"/>
+    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
+      <pane ySplit="600" activePane="bottomLeft"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1039,7 +1038,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>85</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1670,7 +1669,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +1886,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>30</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>30</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>38</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>38</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>38</v>
       </c>
@@ -2147,7 +2146,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>40</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>46</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>49</v>
       </c>
@@ -2487,7 +2486,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>51</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>53</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>57</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>64</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>64</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B95" s="2" t="s">
         <v>85</v>
       </c>
@@ -3104,7 +3103,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>70</v>
       </c>
@@ -3124,7 +3123,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>70</v>
       </c>
@@ -3324,7 +3323,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>53</v>
       </c>
@@ -3345,7 +3344,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>53</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>53</v>
       </c>
@@ -3387,7 +3386,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>76</v>
       </c>
@@ -3408,7 +3407,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>77</v>
       </c>
@@ -3429,7 +3428,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>78</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>93</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>93</v>
       </c>
@@ -4189,7 +4188,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>93</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>93</v>
       </c>
@@ -4235,7 +4234,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>93</v>
       </c>
@@ -4258,7 +4257,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>93</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>93</v>
       </c>
@@ -4304,7 +4303,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>93</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>93</v>
       </c>
@@ -4350,7 +4349,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>93</v>
       </c>
@@ -4373,7 +4372,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>93</v>
       </c>
@@ -4396,7 +4395,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>93</v>
       </c>
@@ -4419,7 +4418,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>93</v>
       </c>
@@ -4442,7 +4441,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>93</v>
       </c>
@@ -4465,7 +4464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>93</v>
       </c>
@@ -4488,7 +4487,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>93</v>
       </c>
@@ -4511,7 +4510,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>93</v>
       </c>
@@ -4531,7 +4530,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>93</v>
       </c>
@@ -4551,7 +4550,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>93</v>
       </c>
@@ -4571,7 +4570,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>93</v>
       </c>
@@ -4594,7 +4593,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>93</v>
       </c>
@@ -4617,7 +4616,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>93</v>
       </c>
@@ -4640,7 +4639,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>94</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>95</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>96</v>
       </c>
@@ -4709,7 +4708,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>97</v>
       </c>
@@ -4732,7 +4731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>98</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>40</v>
       </c>
@@ -4778,7 +4777,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>93</v>
       </c>
@@ -4802,7 +4801,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>93</v>
       </c>
@@ -4826,7 +4825,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>93</v>
       </c>
@@ -4850,7 +4849,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>93</v>
       </c>
@@ -4873,7 +4872,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>93</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>93</v>
       </c>
@@ -4919,7 +4918,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A190"/>
       <c r="B190" t="s">
         <v>100</v>
@@ -4940,7 +4939,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A191"/>
       <c r="B191" t="s">
         <v>100</v>
@@ -4961,7 +4960,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A192"/>
       <c r="B192" t="s">
         <v>100</v>
@@ -4982,7 +4981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A193"/>
       <c r="B193" t="s">
         <v>100</v>
@@ -5003,7 +5002,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>99</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>99</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>99</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>99</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>99</v>
       </c>
@@ -5103,7 +5102,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>99</v>
       </c>
@@ -5123,7 +5122,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>99</v>
       </c>
@@ -5143,7 +5142,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>99</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>99</v>
       </c>
@@ -5183,7 +5182,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>99</v>
       </c>
@@ -5203,7 +5202,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>99</v>
       </c>
@@ -5223,7 +5222,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>99</v>
       </c>
@@ -5243,7 +5242,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>99</v>
       </c>
@@ -5263,7 +5262,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>99</v>
       </c>
@@ -5283,7 +5282,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>93</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" s="2" t="s">
         <v>135</v>
       </c>
@@ -5617,7 +5616,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" s="2" t="s">
         <v>136</v>
       </c>
@@ -5631,7 +5630,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
         <v>137</v>
       </c>
@@ -5645,7 +5644,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" s="2" t="s">
         <v>138</v>
       </c>
@@ -5659,7 +5658,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" s="2" t="s">
         <v>38</v>
       </c>
@@ -5673,7 +5672,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
         <v>38</v>
       </c>
@@ -5687,7 +5686,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>38</v>
       </c>
@@ -5701,7 +5700,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
         <v>139</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A232" s="2" t="s">
         <v>140</v>
       </c>
@@ -5729,7 +5728,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A233" s="2" t="s">
         <v>141</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A234" s="2" t="s">
         <v>142</v>
       </c>
@@ -5757,7 +5756,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
         <v>143</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
         <v>143</v>
       </c>
@@ -5785,7 +5784,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A237" s="2" t="s">
         <v>143</v>
       </c>
@@ -5799,7 +5798,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A238" s="2" t="s">
         <v>70</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
         <v>144</v>
       </c>
@@ -5827,7 +5826,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A240" s="2" t="s">
         <v>64</v>
       </c>
@@ -5841,7 +5840,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" s="2" t="s">
         <v>145</v>
       </c>
@@ -5855,7 +5854,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" s="2" t="s">
         <v>146</v>
       </c>
@@ -5869,7 +5868,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
         <v>147</v>
       </c>
@@ -5927,7 +5926,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" s="2" t="s">
         <v>93</v>
       </c>
@@ -5941,7 +5940,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" s="2" t="s">
         <v>141</v>
       </c>
@@ -5955,7 +5954,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
         <v>38</v>
       </c>
@@ -5969,7 +5968,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" s="2" t="s">
         <v>64</v>
       </c>
@@ -5983,7 +5982,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" s="2" t="s">
         <v>176</v>
       </c>
@@ -6004,7 +6003,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" s="2" t="s">
         <v>177</v>
       </c>
@@ -6025,7 +6024,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
         <v>93</v>
       </c>
@@ -6046,7 +6045,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>152</v>
       </c>
@@ -6060,7 +6059,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>154</v>
       </c>
@@ -6074,7 +6073,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>154</v>
       </c>
@@ -6088,7 +6087,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>154</v>
       </c>
@@ -6102,7 +6101,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>156</v>
       </c>
@@ -6116,7 +6115,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>152</v>
       </c>
@@ -6130,7 +6129,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>157</v>
       </c>
@@ -6144,7 +6143,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>152</v>
       </c>
@@ -6158,7 +6157,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>152</v>
       </c>
@@ -6172,7 +6171,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>152</v>
       </c>
@@ -6186,7 +6185,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>152</v>
       </c>
@@ -6200,7 +6199,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>156</v>
       </c>
@@ -6214,7 +6213,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>157</v>
       </c>
@@ -6228,7 +6227,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>152</v>
       </c>
@@ -6242,7 +6241,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>157</v>
       </c>
@@ -6256,7 +6255,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>152</v>
       </c>
@@ -6270,7 +6269,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>156</v>
       </c>
@@ -6284,7 +6283,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>152</v>
       </c>
@@ -6298,7 +6297,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>157</v>
       </c>
@@ -6312,7 +6311,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>162</v>
       </c>
@@ -6326,7 +6325,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>162</v>
       </c>
@@ -6340,7 +6339,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>164</v>
       </c>
@@ -6354,7 +6353,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>164</v>
       </c>
@@ -6368,7 +6367,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>164</v>
       </c>
@@ -6382,7 +6381,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>165</v>
       </c>
@@ -6396,7 +6395,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>165</v>
       </c>
@@ -6410,7 +6409,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>165</v>
       </c>
@@ -6551,13 +6550,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J287" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Fish"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J287" xr:uid="{9A5ED1FB-7D66-4042-8DC1-3BD3504182B6}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>